<commit_message>
Added date to excel inform
</commit_message>
<xml_diff>
--- a/main/assets/unicode_name.xlsx
+++ b/main/assets/unicode_name.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="57">
   <si>
     <t>Sitio</t>
   </si>
@@ -32,7 +32,157 @@
     <t>Pagina Contacto</t>
   </si>
   <si>
-    <t>http://www.immigrationmiami.com/</t>
+    <t>Ranking Promedio</t>
+  </si>
+  <si>
+    <t>Oppotunity</t>
+  </si>
+  <si>
+    <t>Search Date</t>
+  </si>
+  <si>
+    <t>busqueda relacionada = None</t>
+  </si>
+  <si>
+    <t>https://www.realself.com/</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>You currently rank somewhere in the top 10 on 1 search phrases on Google. If you could land number one spot for all those searches, you'd get about 12132.72 additional clicks per month. That would cost you more than $73691.10 in equivalent PPC dollars.</t>
+  </si>
+  <si>
+    <t>2018-02-02</t>
+  </si>
+  <si>
+    <t>http://www.tamiamidentalcenter.com/</t>
+  </si>
+  <si>
+    <t>https://www.cosmeticdentistrymiami.com/</t>
+  </si>
+  <si>
+    <t>busqueda relacionada = dental implants</t>
+  </si>
+  <si>
+    <t>10 ClearChoice Dental Implants providers near Miami, FL | RealSelf</t>
+  </si>
+  <si>
+    <t>https://www.realself.com/find/Florida/Miami/ClearChoice-Dental-Implants</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>You currently rank somewhere in the top None on None search phrases on Google. If you could land number one spot for all those searches, you'd get about None additional clicks per month. That would cost you more than $None in equivalent PPC dollars.</t>
+  </si>
+  <si>
+    <t>Dental Implants Miami Beach: Cosmetic Dentist - Miami, FL</t>
+  </si>
+  <si>
+    <t>https://www.dentalimplantsmiamibeach.com/</t>
+  </si>
+  <si>
+    <t>Centers for Dental Implants of Miami</t>
+  </si>
+  <si>
+    <t>http://www.gargdmd.com/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(305)935-4991, (954)455-3434 , (954)392-1635 , (305)541-5556 , 3059354991 , (305)935-4991 , (954)455-3434 , (954)392-1635 , (305)541-5556 , (305)935-4991 , (954)455-3434 , (954)392-1635 , (305)541-5556 </t>
+  </si>
+  <si>
+    <t>['miamiimplantsurgeon@gmail.com']</t>
+  </si>
+  <si>
+    <t>http://www.gargdmd.com/contact-us.html</t>
+  </si>
+  <si>
+    <t>New Life Dental: Dental Implants Miami, Florida | Implants for Teeth ...</t>
+  </si>
+  <si>
+    <t>http://www.dentalnewlife.com/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">305-740-1496, 305-740-1496 </t>
+  </si>
+  <si>
+    <t>[]</t>
+  </si>
+  <si>
+    <t>http://www.dentalnewlife.com/contact-us/</t>
+  </si>
+  <si>
+    <t>Dental Implant North Miami FL | Dental Implants Near You</t>
+  </si>
+  <si>
+    <t>http://www.biscaynedentalcenter.com/services/dental-implants/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">305-945-7745, 305-945-7745 , 305-945-7745 , 305-945-7745 , 305-553-9655 </t>
+  </si>
+  <si>
+    <t>http://www.biscaynedentalcenter.com/contact-us/</t>
+  </si>
+  <si>
+    <t>Cosmetic Dentist Miami FL | Miami Center for Cosmetic and Implant ...</t>
+  </si>
+  <si>
+    <t>https://www.miamicosmeticdentalcare.com/</t>
+  </si>
+  <si>
+    <t>Tooth Implants in Coral Gables FL</t>
+  </si>
+  <si>
+    <t>https://www.cosmeticdentistrymiami.com/implant-dentistry.html</t>
+  </si>
+  <si>
+    <t>Dental Implants | Periodontist Dentist &amp; Sedation Dentistry | Miami ...</t>
+  </si>
+  <si>
+    <t>http://www.toothfairyworkshop.com/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(954)963-4700, (954)963-4700 , (954)963-4700 </t>
+  </si>
+  <si>
+    <t>['info@toothfairyworkshop.com']</t>
+  </si>
+  <si>
+    <t>http://www.toothfairyworkshop.com/contact-us/</t>
+  </si>
+  <si>
+    <t>Aventura Dentist | Dentist in Aventura | Hallandale, FL Cosmetic ...</t>
+  </si>
+  <si>
+    <t>http://www.kanedental.com/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(305)466-1444, (305)466-1444 </t>
+  </si>
+  <si>
+    <t>http://www.kanedental.com/contact_information</t>
+  </si>
+  <si>
+    <t>Dental Implants Miami FL | Affordable Doral Dental Implant Cost</t>
+  </si>
+  <si>
+    <t>http://www.dentistmiamisprings.com/dental_implants.php</t>
+  </si>
+  <si>
+    <t>Not Found</t>
+  </si>
+  <si>
+    <t>Miami Beach, Aventura Oral Surgery &amp; Dental Implants</t>
+  </si>
+  <si>
+    <t>http://www.blumnico.com/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">305-538-4556, 305-538-4556 , 305-538-4556 </t>
+  </si>
+  <si>
+    <t>http://www.blumnico.com/contact-us/</t>
   </si>
   <si>
     <t>Direccion</t>
@@ -376,13 +526,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -398,15 +548,337 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="B2" s="1" t="s">
+      <c r="F1" t="s">
         <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="B3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="B4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="B5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G5" t="s">
+        <v>11</v>
+      </c>
+      <c r="H5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F7" t="s">
+        <v>18</v>
+      </c>
+      <c r="G7" t="s">
+        <v>19</v>
+      </c>
+      <c r="H7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F8" t="s">
+        <v>10</v>
+      </c>
+      <c r="G8" t="s">
+        <v>11</v>
+      </c>
+      <c r="H8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9" t="s">
+        <v>25</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F9" t="s">
+        <v>10</v>
+      </c>
+      <c r="G9" t="s">
+        <v>11</v>
+      </c>
+      <c r="H9" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" t="s">
+        <v>29</v>
+      </c>
+      <c r="D10" t="s">
+        <v>30</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F10" t="s">
+        <v>10</v>
+      </c>
+      <c r="G10" t="s">
+        <v>11</v>
+      </c>
+      <c r="H10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" t="s">
+        <v>32</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C11" t="s">
+        <v>34</v>
+      </c>
+      <c r="D11" t="s">
+        <v>30</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F11" t="s">
+        <v>18</v>
+      </c>
+      <c r="G11" t="s">
+        <v>19</v>
+      </c>
+      <c r="H11" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12" t="s">
+        <v>36</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F12" t="s">
+        <v>10</v>
+      </c>
+      <c r="G12" t="s">
+        <v>11</v>
+      </c>
+      <c r="H12" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13" t="s">
+        <v>38</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F13" t="s">
+        <v>18</v>
+      </c>
+      <c r="G13" t="s">
+        <v>19</v>
+      </c>
+      <c r="H13" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14" t="s">
+        <v>40</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C14" t="s">
+        <v>42</v>
+      </c>
+      <c r="D14" t="s">
+        <v>43</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F14" t="s">
+        <v>10</v>
+      </c>
+      <c r="G14" t="s">
+        <v>11</v>
+      </c>
+      <c r="H14" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15" t="s">
+        <v>45</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C15" t="s">
+        <v>47</v>
+      </c>
+      <c r="D15" t="s">
+        <v>30</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F15" t="s">
+        <v>10</v>
+      </c>
+      <c r="G15" t="s">
+        <v>11</v>
+      </c>
+      <c r="H15" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="A16" t="s">
+        <v>49</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D16" t="s">
+        <v>30</v>
+      </c>
+      <c r="E16" t="s">
+        <v>51</v>
+      </c>
+      <c r="F16" t="s">
+        <v>18</v>
+      </c>
+      <c r="G16" t="s">
+        <v>19</v>
+      </c>
+      <c r="H16" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="A17" t="s">
+        <v>52</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C17" t="s">
+        <v>54</v>
+      </c>
+      <c r="D17" t="s">
+        <v>30</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F17" t="s">
+        <v>10</v>
+      </c>
+      <c r="G17" t="s">
+        <v>11</v>
+      </c>
+      <c r="H17" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1"/>
+    <hyperlink ref="B3" r:id="rId1"/>
+    <hyperlink ref="B4" r:id="rId2"/>
+    <hyperlink ref="B5" r:id="rId3"/>
+    <hyperlink ref="B7" r:id="rId4"/>
+    <hyperlink ref="B8" r:id="rId5"/>
+    <hyperlink ref="B9" r:id="rId6"/>
+    <hyperlink ref="E9" r:id="rId7"/>
+    <hyperlink ref="B10" r:id="rId8"/>
+    <hyperlink ref="E10" r:id="rId9"/>
+    <hyperlink ref="B11" r:id="rId10"/>
+    <hyperlink ref="E11" r:id="rId11"/>
+    <hyperlink ref="B12" r:id="rId12"/>
+    <hyperlink ref="B13" r:id="rId13"/>
+    <hyperlink ref="B14" r:id="rId14"/>
+    <hyperlink ref="E14" r:id="rId15"/>
+    <hyperlink ref="B15" r:id="rId16"/>
+    <hyperlink ref="E15" r:id="rId17"/>
+    <hyperlink ref="B16" r:id="rId18"/>
+    <hyperlink ref="B17" r:id="rId19"/>
+    <hyperlink ref="E17" r:id="rId20"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -434,7 +906,7 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>6</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>